<commit_message>
Add duplicate product resolution for bulk product uploads
Adds the duplicate product resolution page for bulk product uploads.
</commit_message>
<xml_diff>
--- a/public/files/PSD High volume product entry Non compliance Form - V1.xlsx
+++ b/public/files/PSD High volume product entry Non compliance Form - V1.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27018"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://beisgov-my.sharepoint.com/personal/sokowoncin_esuga_beis_gov_uk/Documents/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mckeownAd\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC3C3D1E-2743-4D3E-A531-59DAB5DD04B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD70061-370A-4F16-8175-A1F949B71E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{0A922D77-A1EA-4094-9FEA-BA55499A7B85}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0A922D77-A1EA-4094-9FEA-BA55499A7B85}"/>
   </bookViews>
   <sheets>
     <sheet name="Non compliance Form" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028" refMode="R1C1"/>
   <extLst>
@@ -871,7 +871,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1582,29 +1582,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{178542C5-6217-444B-8AE8-8BE71113E419}">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="67" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="2" max="2" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
-    <col min="7" max="7" width="47.5703125" customWidth="1"/>
-    <col min="8" max="8" width="26.42578125" customWidth="1"/>
-    <col min="9" max="9" width="23.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="26.42578125" customWidth="1"/>
-    <col min="11" max="11" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.54296875" customWidth="1"/>
+    <col min="2" max="2" width="32.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.54296875" customWidth="1"/>
+    <col min="4" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7265625" customWidth="1"/>
+    <col min="7" max="7" width="47.54296875" customWidth="1"/>
+    <col min="8" max="8" width="26.453125" customWidth="1"/>
+    <col min="9" max="9" width="23.7265625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="26.453125" customWidth="1"/>
+    <col min="11" max="11" width="38.26953125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="55.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="33.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="55.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="19" customFormat="1" ht="26.25">
+    <row r="1" spans="1:14" s="19" customFormat="1" ht="26" x14ac:dyDescent="0.6">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -1622,7 +1622,7 @@
       <c r="M1" s="23"/>
       <c r="N1" s="23"/>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1666,7 +1666,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1679,7 +1679,7 @@
       <c r="H3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -1692,7 +1692,7 @@
       <c r="H4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -1705,7 +1705,7 @@
       <c r="H5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -1718,139 +1718,139 @@
       <c r="H6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="2:6">
+    <row r="17" spans="2:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="2:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="2:6">
+    <row r="19" spans="2:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="2:6">
+    <row r="20" spans="2:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="2:6">
+    <row r="21" spans="2:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="2:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="2:6">
+    <row r="23" spans="2:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="2:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="2:6">
+    <row r="25" spans="2:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="2:6">
+    <row r="26" spans="2:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="2:6">
+    <row r="27" spans="2:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="2:6">
+    <row r="28" spans="2:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="2:6">
+    <row r="29" spans="2:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -1918,24 +1918,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5396D9AF-C93A-4F29-9C96-200FADF31454}">
   <dimension ref="A1:M199"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
+    <sheetView zoomScale="84" workbookViewId="0">
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="60.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" customWidth="1"/>
-    <col min="11" max="11" width="17.85546875" customWidth="1"/>
-    <col min="13" max="13" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="60.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.7265625" customWidth="1"/>
+    <col min="11" max="11" width="17.81640625" customWidth="1"/>
+    <col min="13" max="13" width="15.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.95" customHeight="1">
+    <row r="1" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="14.45" customHeight="1">
+    <row r="2" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1947,7 +1947,7 @@
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:13" ht="15" thickBot="1">
+    <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1959,7 +1959,7 @@
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
     </row>
-    <row r="4" spans="1:13" ht="15.6" customHeight="1" thickBot="1">
+    <row r="4" spans="1:13" ht="15.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15" thickBot="1">
+    <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15" thickBot="1">
+    <row r="6" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15" thickBot="1">
+    <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15" thickBot="1">
+    <row r="8" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="35.1" customHeight="1" thickBot="1">
+    <row r="9" spans="1:13" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="15" thickBot="1">
+    <row r="10" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15" thickBot="1">
+    <row r="11" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="15" thickBot="1">
+    <row r="12" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -2104,7 +2104,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="15" thickBot="1">
+    <row r="13" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -2122,7 +2122,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="15" thickBot="1">
+    <row r="14" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15" thickBot="1">
+    <row r="15" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -2149,7 +2149,7 @@
       <c r="G15" s="13"/>
       <c r="H15" s="14"/>
     </row>
-    <row r="16" spans="1:13" ht="15" thickBot="1">
+    <row r="16" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>57</v>
       </c>
@@ -2161,7 +2161,7 @@
       <c r="G16" s="14"/>
       <c r="H16" s="13"/>
     </row>
-    <row r="17" spans="1:8" ht="23.45" customHeight="1" thickBot="1">
+    <row r="17" spans="1:8" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>59</v>
       </c>
@@ -2173,7 +2173,7 @@
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
     </row>
-    <row r="18" spans="1:8" ht="15" thickBot="1">
+    <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>61</v>
       </c>
@@ -2185,7 +2185,7 @@
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
     </row>
-    <row r="19" spans="1:8" ht="15" thickBot="1">
+    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>63</v>
       </c>
@@ -2197,7 +2197,7 @@
       <c r="G19" s="13"/>
       <c r="H19" s="14"/>
     </row>
-    <row r="20" spans="1:8" ht="15" thickBot="1">
+    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>65</v>
       </c>
@@ -2209,7 +2209,7 @@
       <c r="G20" s="13"/>
       <c r="H20" s="14"/>
     </row>
-    <row r="21" spans="1:8" ht="15" thickBot="1">
+    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>67</v>
       </c>
@@ -2221,7 +2221,7 @@
       <c r="G21" s="13"/>
       <c r="H21" s="14"/>
     </row>
-    <row r="22" spans="1:8" ht="15" thickBot="1">
+    <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>69</v>
       </c>
@@ -2233,7 +2233,7 @@
       <c r="G22" s="13"/>
       <c r="H22" s="14"/>
     </row>
-    <row r="23" spans="1:8" ht="15" thickBot="1">
+    <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>71</v>
       </c>
@@ -2245,7 +2245,7 @@
       <c r="G23" s="13"/>
       <c r="H23" s="14"/>
     </row>
-    <row r="24" spans="1:8" ht="15" thickBot="1">
+    <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>73</v>
       </c>
@@ -2257,7 +2257,7 @@
       <c r="G24" s="13"/>
       <c r="H24" s="14"/>
     </row>
-    <row r="25" spans="1:8" ht="35.1" customHeight="1" thickBot="1">
+    <row r="25" spans="1:8" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>75</v>
       </c>
@@ -2269,7 +2269,7 @@
       <c r="G25" s="13"/>
       <c r="H25" s="14"/>
     </row>
-    <row r="26" spans="1:8" ht="15" thickBot="1">
+    <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>77</v>
       </c>
@@ -2281,7 +2281,7 @@
       <c r="G26" s="13"/>
       <c r="H26" s="14"/>
     </row>
-    <row r="27" spans="1:8" ht="15" thickBot="1">
+    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>79</v>
       </c>
@@ -2293,7 +2293,7 @@
       <c r="G27" s="13"/>
       <c r="H27" s="14"/>
     </row>
-    <row r="28" spans="1:8" ht="15" thickBot="1">
+    <row r="28" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>81</v>
       </c>
@@ -2305,7 +2305,7 @@
       <c r="G28" s="13"/>
       <c r="H28" s="14"/>
     </row>
-    <row r="29" spans="1:8" ht="15" thickBot="1">
+    <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>83</v>
       </c>
@@ -2317,7 +2317,7 @@
       <c r="G29" s="13"/>
       <c r="H29" s="14"/>
     </row>
-    <row r="30" spans="1:8" ht="23.45" customHeight="1" thickBot="1">
+    <row r="30" spans="1:8" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>85</v>
       </c>
@@ -2329,7 +2329,7 @@
       <c r="G30" s="13"/>
       <c r="H30" s="14"/>
     </row>
-    <row r="31" spans="1:8" ht="15" thickBot="1">
+    <row r="31" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>87</v>
       </c>
@@ -2341,7 +2341,7 @@
       <c r="G31" s="13"/>
       <c r="H31" s="14"/>
     </row>
-    <row r="32" spans="1:8" ht="23.45" customHeight="1" thickBot="1">
+    <row r="32" spans="1:8" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>89</v>
       </c>
@@ -2353,7 +2353,7 @@
       <c r="G32" s="13"/>
       <c r="H32" s="14"/>
     </row>
-    <row r="33" spans="1:8" ht="23.45" customHeight="1" thickBot="1">
+    <row r="33" spans="1:8" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>91</v>
       </c>
@@ -2365,7 +2365,7 @@
       <c r="G33" s="13"/>
       <c r="H33" s="14"/>
     </row>
-    <row r="34" spans="1:8" ht="15" thickBot="1">
+    <row r="34" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>93</v>
       </c>
@@ -2377,7 +2377,7 @@
       <c r="G34" s="13"/>
       <c r="H34" s="14"/>
     </row>
-    <row r="35" spans="1:8" ht="15" thickBot="1">
+    <row r="35" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>95</v>
       </c>
@@ -2389,7 +2389,7 @@
       <c r="G35" s="13"/>
       <c r="H35" s="14"/>
     </row>
-    <row r="36" spans="1:8" ht="15" thickBot="1">
+    <row r="36" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D36" s="10"/>
       <c r="E36" s="11" t="s">
         <v>97</v>
@@ -2398,7 +2398,7 @@
       <c r="G36" s="13"/>
       <c r="H36" s="14"/>
     </row>
-    <row r="37" spans="1:8" ht="35.1" customHeight="1" thickBot="1">
+    <row r="37" spans="1:8" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>98</v>
       </c>
@@ -2410,7 +2410,7 @@
       <c r="G37" s="13"/>
       <c r="H37" s="14"/>
     </row>
-    <row r="38" spans="1:8" ht="15" thickBot="1">
+    <row r="38" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>100</v>
       </c>
@@ -2422,7 +2422,7 @@
       <c r="G38" s="13"/>
       <c r="H38" s="14"/>
     </row>
-    <row r="39" spans="1:8" ht="15" thickBot="1">
+    <row r="39" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="5" t="s">
         <v>102</v>
       </c>
@@ -2434,7 +2434,7 @@
       <c r="G39" s="13"/>
       <c r="H39" s="14"/>
     </row>
-    <row r="40" spans="1:8" ht="15" thickBot="1">
+    <row r="40" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>104</v>
       </c>
@@ -2446,7 +2446,7 @@
       <c r="G40" s="13"/>
       <c r="H40" s="14"/>
     </row>
-    <row r="41" spans="1:8" ht="15" thickBot="1">
+    <row r="41" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>106</v>
       </c>
@@ -2458,7 +2458,7 @@
       <c r="G41" s="13"/>
       <c r="H41" s="14"/>
     </row>
-    <row r="42" spans="1:8" ht="15" thickBot="1">
+    <row r="42" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>108</v>
       </c>
@@ -2470,7 +2470,7 @@
       <c r="G42" s="13"/>
       <c r="H42" s="14"/>
     </row>
-    <row r="43" spans="1:8" ht="46.5" customHeight="1" thickBot="1">
+    <row r="43" spans="1:8" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>110</v>
       </c>
@@ -2482,7 +2482,7 @@
       <c r="G43" s="13"/>
       <c r="H43" s="14"/>
     </row>
-    <row r="44" spans="1:8" ht="15" thickBot="1">
+    <row r="44" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>112</v>
       </c>
@@ -2494,7 +2494,7 @@
       <c r="G44" s="13"/>
       <c r="H44" s="14"/>
     </row>
-    <row r="45" spans="1:8" ht="15" thickBot="1">
+    <row r="45" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>114</v>
       </c>
@@ -2506,7 +2506,7 @@
       <c r="G45" s="13"/>
       <c r="H45" s="14"/>
     </row>
-    <row r="46" spans="1:8" ht="15" thickBot="1">
+    <row r="46" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>116</v>
       </c>
@@ -2518,7 +2518,7 @@
       <c r="G46" s="13"/>
       <c r="H46" s="14"/>
     </row>
-    <row r="47" spans="1:8" ht="15" thickBot="1">
+    <row r="47" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
         <v>118</v>
       </c>
@@ -2530,7 +2530,7 @@
       <c r="G47" s="13"/>
       <c r="H47" s="14"/>
     </row>
-    <row r="48" spans="1:8" ht="35.1" customHeight="1" thickBot="1">
+    <row r="48" spans="1:8" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>120</v>
       </c>
@@ -2542,7 +2542,7 @@
       <c r="G48" s="13"/>
       <c r="H48" s="14"/>
     </row>
-    <row r="49" spans="1:8" ht="46.5" customHeight="1" thickBot="1">
+    <row r="49" spans="1:8" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
         <v>122</v>
       </c>
@@ -2554,7 +2554,7 @@
       <c r="G49" s="13"/>
       <c r="H49" s="14"/>
     </row>
-    <row r="50" spans="1:8" ht="24.6" thickBot="1">
+    <row r="50" spans="1:8" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
         <v>124</v>
       </c>
@@ -2566,7 +2566,7 @@
       <c r="G50" s="13"/>
       <c r="H50" s="14"/>
     </row>
-    <row r="51" spans="1:8" ht="15" thickBot="1">
+    <row r="51" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
         <v>126</v>
       </c>
@@ -2578,7 +2578,7 @@
       <c r="G51" s="13"/>
       <c r="H51" s="14"/>
     </row>
-    <row r="52" spans="1:8" ht="15" thickBot="1">
+    <row r="52" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D52" s="10"/>
       <c r="E52" s="11" t="s">
         <v>128</v>
@@ -2587,7 +2587,7 @@
       <c r="G52" s="14"/>
       <c r="H52" s="14"/>
     </row>
-    <row r="53" spans="1:8" ht="23.45" customHeight="1" thickBot="1">
+    <row r="53" spans="1:8" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D53" s="10"/>
       <c r="E53" s="11" t="s">
         <v>129</v>
@@ -2596,7 +2596,7 @@
       <c r="G53" s="13"/>
       <c r="H53" s="14"/>
     </row>
-    <row r="54" spans="1:8" ht="15" thickBot="1">
+    <row r="54" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D54" s="10"/>
       <c r="E54" s="11" t="s">
         <v>130</v>
@@ -2605,7 +2605,7 @@
       <c r="G54" s="13"/>
       <c r="H54" s="14"/>
     </row>
-    <row r="55" spans="1:8" ht="15" thickBot="1">
+    <row r="55" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D55" s="10"/>
       <c r="E55" s="11" t="s">
         <v>131</v>
@@ -2614,7 +2614,7 @@
       <c r="G55" s="13"/>
       <c r="H55" s="14"/>
     </row>
-    <row r="56" spans="1:8" ht="15" customHeight="1" thickBot="1">
+    <row r="56" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D56" s="10"/>
       <c r="E56" s="11" t="s">
         <v>132</v>
@@ -2623,7 +2623,7 @@
       <c r="G56" s="13"/>
       <c r="H56" s="14"/>
     </row>
-    <row r="57" spans="1:8" ht="23.45" customHeight="1" thickBot="1">
+    <row r="57" spans="1:8" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D57" s="10"/>
       <c r="E57" s="11" t="s">
         <v>133</v>
@@ -2632,7 +2632,7 @@
       <c r="G57" s="13"/>
       <c r="H57" s="14"/>
     </row>
-    <row r="58" spans="1:8" ht="15" thickBot="1">
+    <row r="58" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D58" s="10"/>
       <c r="E58" s="11" t="s">
         <v>134</v>
@@ -2641,7 +2641,7 @@
       <c r="G58" s="13"/>
       <c r="H58" s="14"/>
     </row>
-    <row r="59" spans="1:8" ht="15" thickBot="1">
+    <row r="59" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D59" s="10"/>
       <c r="E59" s="11" t="s">
         <v>135</v>
@@ -2650,7 +2650,7 @@
       <c r="G59" s="13"/>
       <c r="H59" s="14"/>
     </row>
-    <row r="60" spans="1:8" ht="46.5" customHeight="1" thickBot="1">
+    <row r="60" spans="1:8" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D60" s="10"/>
       <c r="E60" s="11" t="s">
         <v>136</v>
@@ -2659,7 +2659,7 @@
       <c r="G60" s="13"/>
       <c r="H60" s="14"/>
     </row>
-    <row r="61" spans="1:8" ht="15" thickBot="1">
+    <row r="61" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D61" s="10"/>
       <c r="E61" s="11" t="s">
         <v>137</v>
@@ -2668,7 +2668,7 @@
       <c r="G61" s="13"/>
       <c r="H61" s="14"/>
     </row>
-    <row r="62" spans="1:8" ht="15" thickBot="1">
+    <row r="62" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D62" s="10"/>
       <c r="E62" s="11" t="s">
         <v>138</v>
@@ -2677,7 +2677,7 @@
       <c r="G62" s="13"/>
       <c r="H62" s="14"/>
     </row>
-    <row r="63" spans="1:8" ht="15" thickBot="1">
+    <row r="63" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D63" s="10"/>
       <c r="E63" s="11" t="s">
         <v>139</v>
@@ -2686,7 +2686,7 @@
       <c r="G63" s="13"/>
       <c r="H63" s="14"/>
     </row>
-    <row r="64" spans="1:8" ht="15" thickBot="1">
+    <row r="64" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D64" s="10"/>
       <c r="E64" s="11" t="s">
         <v>140</v>
@@ -2695,7 +2695,7 @@
       <c r="G64" s="13"/>
       <c r="H64" s="14"/>
     </row>
-    <row r="65" spans="4:8" ht="15" thickBot="1">
+    <row r="65" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D65" s="10"/>
       <c r="E65" s="11" t="s">
         <v>141</v>
@@ -2704,7 +2704,7 @@
       <c r="G65" s="13"/>
       <c r="H65" s="14"/>
     </row>
-    <row r="66" spans="4:8" ht="15" thickBot="1">
+    <row r="66" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D66" s="10"/>
       <c r="E66" s="11" t="s">
         <v>142</v>
@@ -2713,7 +2713,7 @@
       <c r="G66" s="13"/>
       <c r="H66" s="14"/>
     </row>
-    <row r="67" spans="4:8" ht="15" thickBot="1">
+    <row r="67" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D67" s="10"/>
       <c r="E67" s="11" t="s">
         <v>143</v>
@@ -2722,7 +2722,7 @@
       <c r="G67" s="13"/>
       <c r="H67" s="14"/>
     </row>
-    <row r="68" spans="4:8" ht="15" thickBot="1">
+    <row r="68" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D68" s="10"/>
       <c r="E68" s="11" t="s">
         <v>144</v>
@@ -2731,7 +2731,7 @@
       <c r="G68" s="13"/>
       <c r="H68" s="14"/>
     </row>
-    <row r="69" spans="4:8" ht="15" thickBot="1">
+    <row r="69" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D69" s="10"/>
       <c r="E69" s="11" t="s">
         <v>145</v>
@@ -2740,7 +2740,7 @@
       <c r="G69" s="13"/>
       <c r="H69" s="14"/>
     </row>
-    <row r="70" spans="4:8" ht="15" thickBot="1">
+    <row r="70" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D70" s="10"/>
       <c r="E70" s="11" t="s">
         <v>146</v>
@@ -2749,7 +2749,7 @@
       <c r="G70" s="13"/>
       <c r="H70" s="14"/>
     </row>
-    <row r="71" spans="4:8" ht="15" thickBot="1">
+    <row r="71" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D71" s="10"/>
       <c r="E71" s="11" t="s">
         <v>147</v>
@@ -2758,7 +2758,7 @@
       <c r="G71" s="14"/>
       <c r="H71" s="14"/>
     </row>
-    <row r="72" spans="4:8" ht="15" customHeight="1" thickBot="1">
+    <row r="72" spans="4:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D72" s="10"/>
       <c r="E72" s="11" t="s">
         <v>148</v>
@@ -2767,7 +2767,7 @@
       <c r="G72" s="13"/>
       <c r="H72" s="14"/>
     </row>
-    <row r="73" spans="4:8" ht="15" thickBot="1">
+    <row r="73" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D73" s="10"/>
       <c r="E73" s="11" t="s">
         <v>149</v>
@@ -2776,7 +2776,7 @@
       <c r="G73" s="13"/>
       <c r="H73" s="14"/>
     </row>
-    <row r="74" spans="4:8" ht="23.45" customHeight="1" thickBot="1">
+    <row r="74" spans="4:8" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D74" s="10"/>
       <c r="E74" s="11" t="s">
         <v>150</v>
@@ -2785,7 +2785,7 @@
       <c r="G74" s="13"/>
       <c r="H74" s="14"/>
     </row>
-    <row r="75" spans="4:8" ht="15" thickBot="1">
+    <row r="75" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D75" s="10"/>
       <c r="E75" s="11" t="s">
         <v>151</v>
@@ -2794,7 +2794,7 @@
       <c r="G75" s="13"/>
       <c r="H75" s="14"/>
     </row>
-    <row r="76" spans="4:8" ht="15" thickBot="1">
+    <row r="76" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D76" s="10"/>
       <c r="E76" s="11" t="s">
         <v>152</v>
@@ -2803,7 +2803,7 @@
       <c r="G76" s="13"/>
       <c r="H76" s="14"/>
     </row>
-    <row r="77" spans="4:8" ht="15" thickBot="1">
+    <row r="77" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D77" s="10"/>
       <c r="E77" s="11" t="s">
         <v>153</v>
@@ -2812,7 +2812,7 @@
       <c r="G77" s="14"/>
       <c r="H77" s="13"/>
     </row>
-    <row r="78" spans="4:8" ht="15" thickBot="1">
+    <row r="78" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D78" s="10"/>
       <c r="E78" s="11" t="s">
         <v>154</v>
@@ -2821,7 +2821,7 @@
       <c r="G78" s="13"/>
       <c r="H78" s="14"/>
     </row>
-    <row r="79" spans="4:8" ht="15" thickBot="1">
+    <row r="79" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D79" s="10"/>
       <c r="E79" s="11" t="s">
         <v>155</v>
@@ -2830,7 +2830,7 @@
       <c r="G79" s="13"/>
       <c r="H79" s="14"/>
     </row>
-    <row r="80" spans="4:8" ht="15" thickBot="1">
+    <row r="80" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D80" s="10"/>
       <c r="E80" s="11" t="s">
         <v>156</v>
@@ -2839,7 +2839,7 @@
       <c r="G80" s="13"/>
       <c r="H80" s="14"/>
     </row>
-    <row r="81" spans="4:8" ht="15" thickBot="1">
+    <row r="81" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D81" s="10"/>
       <c r="E81" s="11" t="s">
         <v>157</v>
@@ -2848,7 +2848,7 @@
       <c r="G81" s="13"/>
       <c r="H81" s="14"/>
     </row>
-    <row r="82" spans="4:8" ht="15" thickBot="1">
+    <row r="82" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D82" s="10"/>
       <c r="E82" s="11" t="s">
         <v>158</v>
@@ -2857,7 +2857,7 @@
       <c r="G82" s="13"/>
       <c r="H82" s="14"/>
     </row>
-    <row r="83" spans="4:8" ht="15" thickBot="1">
+    <row r="83" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D83" s="10"/>
       <c r="E83" s="11" t="s">
         <v>159</v>
@@ -2866,7 +2866,7 @@
       <c r="G83" s="13"/>
       <c r="H83" s="14"/>
     </row>
-    <row r="84" spans="4:8" ht="15" thickBot="1">
+    <row r="84" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D84" s="10"/>
       <c r="E84" s="11" t="s">
         <v>160</v>
@@ -2875,7 +2875,7 @@
       <c r="G84" s="13"/>
       <c r="H84" s="14"/>
     </row>
-    <row r="85" spans="4:8" ht="15" thickBot="1">
+    <row r="85" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D85" s="10"/>
       <c r="E85" s="11" t="s">
         <v>161</v>
@@ -2884,7 +2884,7 @@
       <c r="G85" s="13"/>
       <c r="H85" s="14"/>
     </row>
-    <row r="86" spans="4:8" ht="15" thickBot="1">
+    <row r="86" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D86" s="10"/>
       <c r="E86" s="11" t="s">
         <v>162</v>
@@ -2893,7 +2893,7 @@
       <c r="G86" s="13"/>
       <c r="H86" s="14"/>
     </row>
-    <row r="87" spans="4:8" ht="15" thickBot="1">
+    <row r="87" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D87" s="10"/>
       <c r="E87" s="11" t="s">
         <v>163</v>
@@ -2902,7 +2902,7 @@
       <c r="G87" s="13"/>
       <c r="H87" s="14"/>
     </row>
-    <row r="88" spans="4:8" ht="15" thickBot="1">
+    <row r="88" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D88" s="10"/>
       <c r="E88" s="11" t="s">
         <v>164</v>
@@ -2911,7 +2911,7 @@
       <c r="G88" s="13"/>
       <c r="H88" s="14"/>
     </row>
-    <row r="89" spans="4:8" ht="15" thickBot="1">
+    <row r="89" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D89" s="10"/>
       <c r="E89" s="11" t="s">
         <v>165</v>
@@ -2920,7 +2920,7 @@
       <c r="G89" s="13"/>
       <c r="H89" s="14"/>
     </row>
-    <row r="90" spans="4:8" ht="15" thickBot="1">
+    <row r="90" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D90" s="10"/>
       <c r="E90" s="11" t="s">
         <v>166</v>
@@ -2929,7 +2929,7 @@
       <c r="G90" s="13"/>
       <c r="H90" s="14"/>
     </row>
-    <row r="91" spans="4:8" ht="15" customHeight="1" thickBot="1">
+    <row r="91" spans="4:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D91" s="10"/>
       <c r="E91" s="11" t="s">
         <v>167</v>
@@ -2938,7 +2938,7 @@
       <c r="G91" s="13"/>
       <c r="H91" s="14"/>
     </row>
-    <row r="92" spans="4:8" ht="15" thickBot="1">
+    <row r="92" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D92" s="10"/>
       <c r="E92" s="11" t="s">
         <v>168</v>
@@ -2947,7 +2947,7 @@
       <c r="G92" s="13"/>
       <c r="H92" s="14"/>
     </row>
-    <row r="93" spans="4:8" ht="15" thickBot="1">
+    <row r="93" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D93" s="10"/>
       <c r="E93" s="11" t="s">
         <v>169</v>
@@ -2956,7 +2956,7 @@
       <c r="G93" s="14"/>
       <c r="H93" s="14"/>
     </row>
-    <row r="94" spans="4:8" ht="15" thickBot="1">
+    <row r="94" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D94" s="10"/>
       <c r="E94" s="11" t="s">
         <v>170</v>
@@ -2965,7 +2965,7 @@
       <c r="G94" s="13"/>
       <c r="H94" s="14"/>
     </row>
-    <row r="95" spans="4:8" ht="15" customHeight="1" thickBot="1">
+    <row r="95" spans="4:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D95" s="10"/>
       <c r="E95" s="11" t="s">
         <v>171</v>
@@ -2974,7 +2974,7 @@
       <c r="G95" s="13"/>
       <c r="H95" s="14"/>
     </row>
-    <row r="96" spans="4:8" ht="15" thickBot="1">
+    <row r="96" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D96" s="10"/>
       <c r="E96" s="11" t="s">
         <v>172</v>
@@ -2983,7 +2983,7 @@
       <c r="G96" s="13"/>
       <c r="H96" s="14"/>
     </row>
-    <row r="97" spans="4:8" ht="15" thickBot="1">
+    <row r="97" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D97" s="10"/>
       <c r="E97" s="11" t="s">
         <v>173</v>
@@ -2992,7 +2992,7 @@
       <c r="G97" s="13"/>
       <c r="H97" s="14"/>
     </row>
-    <row r="98" spans="4:8" ht="15" thickBot="1">
+    <row r="98" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D98" s="10"/>
       <c r="E98" s="11" t="s">
         <v>174</v>
@@ -3001,7 +3001,7 @@
       <c r="G98" s="13"/>
       <c r="H98" s="14"/>
     </row>
-    <row r="99" spans="4:8" ht="15" thickBot="1">
+    <row r="99" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D99" s="10"/>
       <c r="E99" s="11" t="s">
         <v>175</v>
@@ -3010,7 +3010,7 @@
       <c r="G99" s="13"/>
       <c r="H99" s="14"/>
     </row>
-    <row r="100" spans="4:8" ht="15" thickBot="1">
+    <row r="100" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D100" s="10"/>
       <c r="E100" s="11" t="s">
         <v>176</v>
@@ -3019,7 +3019,7 @@
       <c r="G100" s="13"/>
       <c r="H100" s="14"/>
     </row>
-    <row r="101" spans="4:8" ht="15" thickBot="1">
+    <row r="101" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D101" s="10"/>
       <c r="E101" s="11" t="s">
         <v>177</v>
@@ -3028,7 +3028,7 @@
       <c r="G101" s="13"/>
       <c r="H101" s="14"/>
     </row>
-    <row r="102" spans="4:8" ht="23.45" customHeight="1" thickBot="1">
+    <row r="102" spans="4:8" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D102" s="10"/>
       <c r="E102" s="11" t="s">
         <v>178</v>
@@ -3037,7 +3037,7 @@
       <c r="G102" s="14"/>
       <c r="H102" s="14"/>
     </row>
-    <row r="103" spans="4:8" ht="15" thickBot="1">
+    <row r="103" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D103" s="10"/>
       <c r="E103" s="11" t="s">
         <v>179</v>
@@ -3046,7 +3046,7 @@
       <c r="G103" s="13"/>
       <c r="H103" s="14"/>
     </row>
-    <row r="104" spans="4:8" ht="23.45" customHeight="1" thickBot="1">
+    <row r="104" spans="4:8" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D104" s="10"/>
       <c r="E104" s="11" t="s">
         <v>180</v>
@@ -3055,7 +3055,7 @@
       <c r="G104" s="13"/>
       <c r="H104" s="14"/>
     </row>
-    <row r="105" spans="4:8" ht="23.45" customHeight="1" thickBot="1">
+    <row r="105" spans="4:8" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D105" s="10"/>
       <c r="E105" s="11" t="s">
         <v>181</v>
@@ -3064,7 +3064,7 @@
       <c r="G105" s="13"/>
       <c r="H105" s="14"/>
     </row>
-    <row r="106" spans="4:8" ht="15" thickBot="1">
+    <row r="106" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D106" s="10"/>
       <c r="E106" s="11" t="s">
         <v>182</v>
@@ -3073,7 +3073,7 @@
       <c r="G106" s="13"/>
       <c r="H106" s="14"/>
     </row>
-    <row r="107" spans="4:8" ht="15" thickBot="1">
+    <row r="107" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D107" s="10"/>
       <c r="E107" s="11" t="s">
         <v>183</v>
@@ -3082,7 +3082,7 @@
       <c r="G107" s="13"/>
       <c r="H107" s="14"/>
     </row>
-    <row r="108" spans="4:8" ht="15" thickBot="1">
+    <row r="108" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D108" s="10"/>
       <c r="E108" s="11" t="s">
         <v>184</v>
@@ -3091,7 +3091,7 @@
       <c r="G108" s="14"/>
       <c r="H108" s="13"/>
     </row>
-    <row r="109" spans="4:8" ht="15" thickBot="1">
+    <row r="109" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D109" s="10"/>
       <c r="E109" s="11" t="s">
         <v>185</v>
@@ -3100,7 +3100,7 @@
       <c r="G109" s="13"/>
       <c r="H109" s="14"/>
     </row>
-    <row r="110" spans="4:8" ht="15" thickBot="1">
+    <row r="110" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D110" s="10"/>
       <c r="E110" s="11" t="s">
         <v>186</v>
@@ -3109,7 +3109,7 @@
       <c r="G110" s="14"/>
       <c r="H110" s="13"/>
     </row>
-    <row r="111" spans="4:8" ht="23.45" customHeight="1" thickBot="1">
+    <row r="111" spans="4:8" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D111" s="10"/>
       <c r="E111" s="11" t="s">
         <v>187</v>
@@ -3118,7 +3118,7 @@
       <c r="G111" s="14"/>
       <c r="H111" s="14"/>
     </row>
-    <row r="112" spans="4:8" ht="15" customHeight="1" thickBot="1">
+    <row r="112" spans="4:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D112" s="10"/>
       <c r="E112" s="11" t="s">
         <v>188</v>
@@ -3127,7 +3127,7 @@
       <c r="G112" s="13"/>
       <c r="H112" s="14"/>
     </row>
-    <row r="113" spans="4:8" ht="15" thickBot="1">
+    <row r="113" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D113" s="10"/>
       <c r="E113" s="11" t="s">
         <v>189</v>
@@ -3136,7 +3136,7 @@
       <c r="G113" s="13"/>
       <c r="H113" s="14"/>
     </row>
-    <row r="114" spans="4:8" ht="15" thickBot="1">
+    <row r="114" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D114" s="10"/>
       <c r="E114" s="11" t="s">
         <v>190</v>
@@ -3145,7 +3145,7 @@
       <c r="G114" s="13"/>
       <c r="H114" s="14"/>
     </row>
-    <row r="115" spans="4:8" ht="15" customHeight="1" thickBot="1">
+    <row r="115" spans="4:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D115" s="10"/>
       <c r="E115" s="11" t="s">
         <v>191</v>
@@ -3154,7 +3154,7 @@
       <c r="G115" s="14"/>
       <c r="H115" s="14"/>
     </row>
-    <row r="116" spans="4:8" ht="15" thickBot="1">
+    <row r="116" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D116" s="10"/>
       <c r="E116" s="11" t="s">
         <v>192</v>
@@ -3163,7 +3163,7 @@
       <c r="G116" s="13"/>
       <c r="H116" s="14"/>
     </row>
-    <row r="117" spans="4:8" ht="15" thickBot="1">
+    <row r="117" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D117" s="10"/>
       <c r="E117" s="11" t="s">
         <v>193</v>
@@ -3172,7 +3172,7 @@
       <c r="G117" s="14"/>
       <c r="H117" s="13"/>
     </row>
-    <row r="118" spans="4:8" ht="15" thickBot="1">
+    <row r="118" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D118" s="10"/>
       <c r="E118" s="11" t="s">
         <v>194</v>
@@ -3181,7 +3181,7 @@
       <c r="G118" s="13"/>
       <c r="H118" s="14"/>
     </row>
-    <row r="119" spans="4:8" ht="23.45" customHeight="1" thickBot="1">
+    <row r="119" spans="4:8" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D119" s="10"/>
       <c r="E119" s="11" t="s">
         <v>195</v>
@@ -3190,7 +3190,7 @@
       <c r="G119" s="13"/>
       <c r="H119" s="14"/>
     </row>
-    <row r="120" spans="4:8" ht="15" thickBot="1">
+    <row r="120" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D120" s="10"/>
       <c r="E120" s="11" t="s">
         <v>196</v>
@@ -3199,7 +3199,7 @@
       <c r="G120" s="13"/>
       <c r="H120" s="14"/>
     </row>
-    <row r="121" spans="4:8" ht="23.45" customHeight="1" thickBot="1">
+    <row r="121" spans="4:8" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D121" s="10"/>
       <c r="E121" s="11" t="s">
         <v>197</v>
@@ -3208,7 +3208,7 @@
       <c r="G121" s="13"/>
       <c r="H121" s="14"/>
     </row>
-    <row r="122" spans="4:8" ht="35.1" customHeight="1" thickBot="1">
+    <row r="122" spans="4:8" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D122" s="10"/>
       <c r="E122" s="11" t="s">
         <v>198</v>
@@ -3217,7 +3217,7 @@
       <c r="G122" s="13"/>
       <c r="H122" s="14"/>
     </row>
-    <row r="123" spans="4:8" ht="15" thickBot="1">
+    <row r="123" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D123" s="10"/>
       <c r="E123" s="11" t="s">
         <v>199</v>
@@ -3226,7 +3226,7 @@
       <c r="G123" s="13"/>
       <c r="H123" s="14"/>
     </row>
-    <row r="124" spans="4:8" ht="15" thickBot="1">
+    <row r="124" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D124" s="10"/>
       <c r="E124" s="11" t="s">
         <v>200</v>
@@ -3235,7 +3235,7 @@
       <c r="G124" s="14"/>
       <c r="H124" s="14"/>
     </row>
-    <row r="125" spans="4:8" ht="15" thickBot="1">
+    <row r="125" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D125" s="10"/>
       <c r="E125" s="11" t="s">
         <v>201</v>
@@ -3244,7 +3244,7 @@
       <c r="G125" s="13"/>
       <c r="H125" s="14"/>
     </row>
-    <row r="126" spans="4:8" ht="23.45" customHeight="1" thickBot="1">
+    <row r="126" spans="4:8" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D126" s="10"/>
       <c r="E126" s="11" t="s">
         <v>202</v>
@@ -3253,7 +3253,7 @@
       <c r="G126" s="13"/>
       <c r="H126" s="14"/>
     </row>
-    <row r="127" spans="4:8" ht="23.45" customHeight="1" thickBot="1">
+    <row r="127" spans="4:8" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D127" s="10"/>
       <c r="E127" s="11" t="s">
         <v>203</v>
@@ -3262,7 +3262,7 @@
       <c r="G127" s="13"/>
       <c r="H127" s="14"/>
     </row>
-    <row r="128" spans="4:8" ht="15" thickBot="1">
+    <row r="128" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D128" s="10"/>
       <c r="E128" s="11" t="s">
         <v>204</v>
@@ -3271,7 +3271,7 @@
       <c r="G128" s="13"/>
       <c r="H128" s="14"/>
     </row>
-    <row r="129" spans="4:8" ht="15" thickBot="1">
+    <row r="129" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D129" s="10"/>
       <c r="E129" s="11" t="s">
         <v>205</v>
@@ -3280,7 +3280,7 @@
       <c r="G129" s="13"/>
       <c r="H129" s="14"/>
     </row>
-    <row r="130" spans="4:8" ht="15" thickBot="1">
+    <row r="130" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D130" s="10"/>
       <c r="E130" s="11" t="s">
         <v>206</v>
@@ -3289,7 +3289,7 @@
       <c r="G130" s="13"/>
       <c r="H130" s="14"/>
     </row>
-    <row r="131" spans="4:8" ht="23.45" customHeight="1" thickBot="1">
+    <row r="131" spans="4:8" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D131" s="10"/>
       <c r="E131" s="11" t="s">
         <v>207</v>
@@ -3298,7 +3298,7 @@
       <c r="G131" s="13"/>
       <c r="H131" s="14"/>
     </row>
-    <row r="132" spans="4:8" ht="23.45" customHeight="1" thickBot="1">
+    <row r="132" spans="4:8" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D132" s="10"/>
       <c r="E132" s="11" t="s">
         <v>208</v>
@@ -3307,7 +3307,7 @@
       <c r="G132" s="13"/>
       <c r="H132" s="14"/>
     </row>
-    <row r="133" spans="4:8" ht="15" thickBot="1">
+    <row r="133" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D133" s="10"/>
       <c r="E133" s="11" t="s">
         <v>209</v>
@@ -3316,7 +3316,7 @@
       <c r="G133" s="13"/>
       <c r="H133" s="14"/>
     </row>
-    <row r="134" spans="4:8" ht="15" thickBot="1">
+    <row r="134" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D134" s="10"/>
       <c r="E134" s="11" t="s">
         <v>210</v>
@@ -3325,7 +3325,7 @@
       <c r="G134" s="13"/>
       <c r="H134" s="14"/>
     </row>
-    <row r="135" spans="4:8" ht="15" thickBot="1">
+    <row r="135" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D135" s="10"/>
       <c r="E135" s="11" t="s">
         <v>211</v>
@@ -3334,7 +3334,7 @@
       <c r="G135" s="13"/>
       <c r="H135" s="14"/>
     </row>
-    <row r="136" spans="4:8" ht="15" thickBot="1">
+    <row r="136" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D136" s="10"/>
       <c r="E136" s="11" t="s">
         <v>212</v>
@@ -3343,7 +3343,7 @@
       <c r="G136" s="14"/>
       <c r="H136" s="14"/>
     </row>
-    <row r="137" spans="4:8" ht="23.45" customHeight="1" thickBot="1">
+    <row r="137" spans="4:8" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D137" s="10"/>
       <c r="E137" s="11" t="s">
         <v>213</v>
@@ -3352,7 +3352,7 @@
       <c r="G137" s="13"/>
       <c r="H137" s="14"/>
     </row>
-    <row r="138" spans="4:8" ht="15" thickBot="1">
+    <row r="138" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D138" s="10"/>
       <c r="E138" s="11" t="s">
         <v>214</v>
@@ -3361,7 +3361,7 @@
       <c r="G138" s="13"/>
       <c r="H138" s="14"/>
     </row>
-    <row r="139" spans="4:8" ht="23.45" customHeight="1" thickBot="1">
+    <row r="139" spans="4:8" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D139" s="10"/>
       <c r="E139" s="11" t="s">
         <v>215</v>
@@ -3370,7 +3370,7 @@
       <c r="G139" s="13"/>
       <c r="H139" s="14"/>
     </row>
-    <row r="140" spans="4:8" ht="15" thickBot="1">
+    <row r="140" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D140" s="10"/>
       <c r="E140" s="11" t="s">
         <v>216</v>
@@ -3379,7 +3379,7 @@
       <c r="G140" s="13"/>
       <c r="H140" s="14"/>
     </row>
-    <row r="141" spans="4:8" ht="15" thickBot="1">
+    <row r="141" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D141" s="10"/>
       <c r="E141" s="11" t="s">
         <v>217</v>
@@ -3388,7 +3388,7 @@
       <c r="G141" s="13"/>
       <c r="H141" s="14"/>
     </row>
-    <row r="142" spans="4:8" ht="15" customHeight="1" thickBot="1">
+    <row r="142" spans="4:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D142" s="10"/>
       <c r="E142" s="11" t="s">
         <v>218</v>
@@ -3397,7 +3397,7 @@
       <c r="G142" s="13"/>
       <c r="H142" s="14"/>
     </row>
-    <row r="143" spans="4:8" ht="15" thickBot="1">
+    <row r="143" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D143" s="10"/>
       <c r="E143" s="11" t="s">
         <v>219</v>
@@ -3406,7 +3406,7 @@
       <c r="G143" s="13"/>
       <c r="H143" s="14"/>
     </row>
-    <row r="144" spans="4:8" ht="15" thickBot="1">
+    <row r="144" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D144" s="10"/>
       <c r="E144" s="11" t="s">
         <v>220</v>
@@ -3415,7 +3415,7 @@
       <c r="G144" s="13"/>
       <c r="H144" s="14"/>
     </row>
-    <row r="145" spans="4:8" ht="15" thickBot="1">
+    <row r="145" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D145" s="10"/>
       <c r="E145" s="11" t="s">
         <v>221</v>
@@ -3424,7 +3424,7 @@
       <c r="G145" s="13"/>
       <c r="H145" s="14"/>
     </row>
-    <row r="146" spans="4:8" ht="15" thickBot="1">
+    <row r="146" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D146" s="10"/>
       <c r="E146" s="11" t="s">
         <v>222</v>
@@ -3433,7 +3433,7 @@
       <c r="G146" s="13"/>
       <c r="H146" s="14"/>
     </row>
-    <row r="147" spans="4:8" ht="15" thickBot="1">
+    <row r="147" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D147" s="10"/>
       <c r="E147" s="11" t="s">
         <v>223</v>
@@ -3442,7 +3442,7 @@
       <c r="G147" s="13"/>
       <c r="H147" s="14"/>
     </row>
-    <row r="148" spans="4:8" ht="15" thickBot="1">
+    <row r="148" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D148" s="10"/>
       <c r="E148" s="11" t="s">
         <v>224</v>
@@ -3451,7 +3451,7 @@
       <c r="G148" s="13"/>
       <c r="H148" s="14"/>
     </row>
-    <row r="149" spans="4:8" ht="23.45" customHeight="1" thickBot="1">
+    <row r="149" spans="4:8" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D149" s="10"/>
       <c r="E149" s="11" t="s">
         <v>225</v>
@@ -3460,7 +3460,7 @@
       <c r="G149" s="14"/>
       <c r="H149" s="14"/>
     </row>
-    <row r="150" spans="4:8" ht="15" customHeight="1" thickBot="1">
+    <row r="150" spans="4:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D150" s="10"/>
       <c r="E150" s="11" t="s">
         <v>226</v>
@@ -3469,7 +3469,7 @@
       <c r="G150" s="14"/>
       <c r="H150" s="14"/>
     </row>
-    <row r="151" spans="4:8" ht="46.5" customHeight="1" thickBot="1">
+    <row r="151" spans="4:8" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D151" s="10"/>
       <c r="E151" s="11" t="s">
         <v>227</v>
@@ -3478,7 +3478,7 @@
       <c r="G151" s="14"/>
       <c r="H151" s="14"/>
     </row>
-    <row r="152" spans="4:8" ht="24.6" thickBot="1">
+    <row r="152" spans="4:8" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D152" s="10"/>
       <c r="E152" s="11" t="s">
         <v>228</v>
@@ -3487,7 +3487,7 @@
       <c r="G152" s="13"/>
       <c r="H152" s="14"/>
     </row>
-    <row r="153" spans="4:8" ht="15" customHeight="1" thickBot="1">
+    <row r="153" spans="4:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D153" s="10"/>
       <c r="E153" s="11" t="s">
         <v>229</v>
@@ -3496,7 +3496,7 @@
       <c r="G153" s="14"/>
       <c r="H153" s="14"/>
     </row>
-    <row r="154" spans="4:8" ht="35.1" customHeight="1" thickBot="1">
+    <row r="154" spans="4:8" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D154" s="10"/>
       <c r="E154" s="11" t="s">
         <v>230</v>
@@ -3505,7 +3505,7 @@
       <c r="G154" s="14"/>
       <c r="H154" s="14"/>
     </row>
-    <row r="155" spans="4:8" ht="23.45" customHeight="1" thickBot="1">
+    <row r="155" spans="4:8" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D155" s="10"/>
       <c r="E155" s="11" t="s">
         <v>231</v>
@@ -3514,7 +3514,7 @@
       <c r="G155" s="13"/>
       <c r="H155" s="14"/>
     </row>
-    <row r="156" spans="4:8" ht="15" thickBot="1">
+    <row r="156" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D156" s="10"/>
       <c r="E156" s="11" t="s">
         <v>232</v>
@@ -3523,7 +3523,7 @@
       <c r="G156" s="13"/>
       <c r="H156" s="14"/>
     </row>
-    <row r="157" spans="4:8" ht="15" thickBot="1">
+    <row r="157" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D157" s="10"/>
       <c r="E157" s="11" t="s">
         <v>233</v>
@@ -3532,7 +3532,7 @@
       <c r="G157" s="13"/>
       <c r="H157" s="14"/>
     </row>
-    <row r="158" spans="4:8" ht="15" thickBot="1">
+    <row r="158" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D158" s="10"/>
       <c r="E158" s="11" t="s">
         <v>234</v>
@@ -3541,7 +3541,7 @@
       <c r="G158" s="14"/>
       <c r="H158" s="14"/>
     </row>
-    <row r="159" spans="4:8" ht="23.45" customHeight="1" thickBot="1">
+    <row r="159" spans="4:8" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D159" s="10"/>
       <c r="E159" s="11" t="s">
         <v>235</v>
@@ -3550,7 +3550,7 @@
       <c r="G159" s="13"/>
       <c r="H159" s="14"/>
     </row>
-    <row r="160" spans="4:8" ht="15" thickBot="1">
+    <row r="160" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D160" s="10"/>
       <c r="E160" s="11" t="s">
         <v>236</v>
@@ -3559,7 +3559,7 @@
       <c r="G160" s="14"/>
       <c r="H160" s="13"/>
     </row>
-    <row r="161" spans="4:8" ht="15" thickBot="1">
+    <row r="161" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D161" s="10"/>
       <c r="E161" s="11" t="s">
         <v>237</v>
@@ -3568,7 +3568,7 @@
       <c r="G161" s="13"/>
       <c r="H161" s="14"/>
     </row>
-    <row r="162" spans="4:8" ht="15" thickBot="1">
+    <row r="162" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D162" s="10"/>
       <c r="E162" s="11" t="s">
         <v>238</v>
@@ -3577,7 +3577,7 @@
       <c r="G162" s="13"/>
       <c r="H162" s="14"/>
     </row>
-    <row r="163" spans="4:8" ht="23.45" customHeight="1" thickBot="1">
+    <row r="163" spans="4:8" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D163" s="10"/>
       <c r="E163" s="11" t="s">
         <v>239</v>
@@ -3586,7 +3586,7 @@
       <c r="G163" s="13"/>
       <c r="H163" s="14"/>
     </row>
-    <row r="164" spans="4:8" ht="15" thickBot="1">
+    <row r="164" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D164" s="10"/>
       <c r="E164" s="11" t="s">
         <v>240</v>
@@ -3595,7 +3595,7 @@
       <c r="G164" s="13"/>
       <c r="H164" s="14"/>
     </row>
-    <row r="165" spans="4:8" ht="23.45" customHeight="1" thickBot="1">
+    <row r="165" spans="4:8" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D165" s="10"/>
       <c r="E165" s="11" t="s">
         <v>241</v>
@@ -3604,7 +3604,7 @@
       <c r="G165" s="13"/>
       <c r="H165" s="14"/>
     </row>
-    <row r="166" spans="4:8" ht="23.45" customHeight="1" thickBot="1">
+    <row r="166" spans="4:8" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D166" s="10"/>
       <c r="E166" s="11" t="s">
         <v>242</v>
@@ -3613,7 +3613,7 @@
       <c r="G166" s="13"/>
       <c r="H166" s="14"/>
     </row>
-    <row r="167" spans="4:8" ht="23.45" customHeight="1" thickBot="1">
+    <row r="167" spans="4:8" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D167" s="10"/>
       <c r="E167" s="11" t="s">
         <v>243</v>
@@ -3622,7 +3622,7 @@
       <c r="G167" s="13"/>
       <c r="H167" s="14"/>
     </row>
-    <row r="168" spans="4:8" ht="15" thickBot="1">
+    <row r="168" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D168" s="10"/>
       <c r="E168" s="11" t="s">
         <v>244</v>
@@ -3631,7 +3631,7 @@
       <c r="G168" s="13"/>
       <c r="H168" s="14"/>
     </row>
-    <row r="169" spans="4:8" ht="15" thickBot="1">
+    <row r="169" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D169" s="10"/>
       <c r="E169" s="11" t="s">
         <v>245</v>
@@ -3640,7 +3640,7 @@
       <c r="G169" s="13"/>
       <c r="H169" s="14"/>
     </row>
-    <row r="170" spans="4:8" ht="15" thickBot="1">
+    <row r="170" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D170" s="10"/>
       <c r="E170" s="11" t="s">
         <v>246</v>
@@ -3649,7 +3649,7 @@
       <c r="G170" s="13"/>
       <c r="H170" s="14"/>
     </row>
-    <row r="171" spans="4:8" ht="15" thickBot="1">
+    <row r="171" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D171" s="10"/>
       <c r="E171" s="11" t="s">
         <v>247</v>
@@ -3658,7 +3658,7 @@
       <c r="G171" s="13"/>
       <c r="H171" s="14"/>
     </row>
-    <row r="172" spans="4:8" ht="15" thickBot="1">
+    <row r="172" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D172" s="10"/>
       <c r="E172" s="11" t="s">
         <v>248</v>
@@ -3667,7 +3667,7 @@
       <c r="G172" s="13"/>
       <c r="H172" s="14"/>
     </row>
-    <row r="173" spans="4:8" ht="23.45" customHeight="1" thickBot="1">
+    <row r="173" spans="4:8" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D173" s="10"/>
       <c r="E173" s="11" t="s">
         <v>249</v>
@@ -3676,7 +3676,7 @@
       <c r="G173" s="13"/>
       <c r="H173" s="14"/>
     </row>
-    <row r="174" spans="4:8" ht="15" thickBot="1">
+    <row r="174" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D174" s="10"/>
       <c r="E174" s="11" t="s">
         <v>250</v>
@@ -3685,7 +3685,7 @@
       <c r="G174" s="13"/>
       <c r="H174" s="14"/>
     </row>
-    <row r="175" spans="4:8" ht="15" thickBot="1">
+    <row r="175" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D175" s="10"/>
       <c r="E175" s="11" t="s">
         <v>251</v>
@@ -3694,7 +3694,7 @@
       <c r="G175" s="13"/>
       <c r="H175" s="14"/>
     </row>
-    <row r="176" spans="4:8" ht="15" thickBot="1">
+    <row r="176" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D176" s="10"/>
       <c r="E176" s="11" t="s">
         <v>252</v>
@@ -3703,7 +3703,7 @@
       <c r="G176" s="13"/>
       <c r="H176" s="14"/>
     </row>
-    <row r="177" spans="4:8" ht="15" thickBot="1">
+    <row r="177" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D177" s="10"/>
       <c r="E177" s="11" t="s">
         <v>253</v>
@@ -3712,7 +3712,7 @@
       <c r="G177" s="13"/>
       <c r="H177" s="14"/>
     </row>
-    <row r="178" spans="4:8" ht="23.45" customHeight="1" thickBot="1">
+    <row r="178" spans="4:8" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D178" s="10"/>
       <c r="E178" s="11" t="s">
         <v>254</v>
@@ -3721,7 +3721,7 @@
       <c r="G178" s="13"/>
       <c r="H178" s="14"/>
     </row>
-    <row r="179" spans="4:8" ht="15" thickBot="1">
+    <row r="179" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D179" s="10"/>
       <c r="E179" s="11" t="s">
         <v>255</v>
@@ -3730,7 +3730,7 @@
       <c r="G179" s="13"/>
       <c r="H179" s="14"/>
     </row>
-    <row r="180" spans="4:8" ht="15" thickBot="1">
+    <row r="180" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D180" s="10"/>
       <c r="E180" s="11" t="s">
         <v>256</v>
@@ -3739,7 +3739,7 @@
       <c r="G180" s="14"/>
       <c r="H180" s="14"/>
     </row>
-    <row r="181" spans="4:8" ht="35.1" customHeight="1" thickBot="1">
+    <row r="181" spans="4:8" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D181" s="10"/>
       <c r="E181" s="11" t="s">
         <v>257</v>
@@ -3748,7 +3748,7 @@
       <c r="G181" s="13"/>
       <c r="H181" s="14"/>
     </row>
-    <row r="182" spans="4:8" ht="15" thickBot="1">
+    <row r="182" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D182" s="10"/>
       <c r="E182" s="11" t="s">
         <v>258</v>
@@ -3757,7 +3757,7 @@
       <c r="G182" s="13"/>
       <c r="H182" s="14"/>
     </row>
-    <row r="183" spans="4:8" ht="15" thickBot="1">
+    <row r="183" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D183" s="10"/>
       <c r="E183" s="11" t="s">
         <v>259</v>
@@ -3766,7 +3766,7 @@
       <c r="G183" s="13"/>
       <c r="H183" s="14"/>
     </row>
-    <row r="184" spans="4:8" ht="23.45" customHeight="1" thickBot="1">
+    <row r="184" spans="4:8" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D184" s="10"/>
       <c r="E184" s="11" t="s">
         <v>260</v>
@@ -3775,7 +3775,7 @@
       <c r="G184" s="13"/>
       <c r="H184" s="14"/>
     </row>
-    <row r="185" spans="4:8" ht="15" thickBot="1">
+    <row r="185" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D185" s="10"/>
       <c r="E185" s="11" t="s">
         <v>261</v>
@@ -3784,7 +3784,7 @@
       <c r="G185" s="14"/>
       <c r="H185" s="14"/>
     </row>
-    <row r="186" spans="4:8" ht="15" thickBot="1">
+    <row r="186" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D186" s="10"/>
       <c r="E186" s="11" t="s">
         <v>262</v>
@@ -3793,7 +3793,7 @@
       <c r="G186" s="13"/>
       <c r="H186" s="14"/>
     </row>
-    <row r="187" spans="4:8" ht="15" thickBot="1">
+    <row r="187" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D187" s="10"/>
       <c r="E187" s="11" t="s">
         <v>263</v>
@@ -3802,7 +3802,7 @@
       <c r="G187" s="13"/>
       <c r="H187" s="14"/>
     </row>
-    <row r="188" spans="4:8" ht="35.1" customHeight="1" thickBot="1">
+    <row r="188" spans="4:8" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D188" s="10"/>
       <c r="E188" s="11" t="s">
         <v>264</v>
@@ -3811,7 +3811,7 @@
       <c r="G188" s="13"/>
       <c r="H188" s="14"/>
     </row>
-    <row r="189" spans="4:8" ht="23.45" customHeight="1" thickBot="1">
+    <row r="189" spans="4:8" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D189" s="10"/>
       <c r="E189" s="11" t="s">
         <v>265</v>
@@ -3820,7 +3820,7 @@
       <c r="G189" s="13"/>
       <c r="H189" s="14"/>
     </row>
-    <row r="190" spans="4:8" ht="35.1" customHeight="1" thickBot="1">
+    <row r="190" spans="4:8" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D190" s="10"/>
       <c r="E190" s="11" t="s">
         <v>266</v>
@@ -3829,7 +3829,7 @@
       <c r="G190" s="13"/>
       <c r="H190" s="14"/>
     </row>
-    <row r="191" spans="4:8" ht="15" thickBot="1">
+    <row r="191" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D191" s="10"/>
       <c r="E191" s="11" t="s">
         <v>267</v>
@@ -3838,7 +3838,7 @@
       <c r="G191" s="13"/>
       <c r="H191" s="14"/>
     </row>
-    <row r="192" spans="4:8" ht="15" customHeight="1" thickBot="1">
+    <row r="192" spans="4:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D192" s="10"/>
       <c r="E192" s="11" t="s">
         <v>268</v>
@@ -3847,7 +3847,7 @@
       <c r="G192" s="13"/>
       <c r="H192" s="14"/>
     </row>
-    <row r="193" spans="4:8" ht="15" thickBot="1">
+    <row r="193" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D193" s="10"/>
       <c r="E193" s="11" t="s">
         <v>269</v>
@@ -3856,7 +3856,7 @@
       <c r="G193" s="13"/>
       <c r="H193" s="14"/>
     </row>
-    <row r="194" spans="4:8" ht="15" thickBot="1">
+    <row r="194" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D194" s="10"/>
       <c r="E194" s="11" t="s">
         <v>270</v>
@@ -3865,7 +3865,7 @@
       <c r="G194" s="13"/>
       <c r="H194" s="14"/>
     </row>
-    <row r="195" spans="4:8" ht="15" thickBot="1">
+    <row r="195" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D195" s="10"/>
       <c r="E195" s="11" t="s">
         <v>271</v>
@@ -3874,7 +3874,7 @@
       <c r="G195" s="13"/>
       <c r="H195" s="14"/>
     </row>
-    <row r="196" spans="4:8" ht="15" thickBot="1">
+    <row r="196" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D196" s="10"/>
       <c r="E196" s="11" t="s">
         <v>272</v>
@@ -3883,7 +3883,7 @@
       <c r="G196" s="13"/>
       <c r="H196" s="14"/>
     </row>
-    <row r="197" spans="4:8" ht="15" thickBot="1">
+    <row r="197" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D197" s="10"/>
       <c r="E197" s="11" t="s">
         <v>273</v>
@@ -3892,7 +3892,7 @@
       <c r="G197" s="13"/>
       <c r="H197" s="14"/>
     </row>
-    <row r="198" spans="4:8" ht="15" thickBot="1">
+    <row r="198" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D198" s="16"/>
       <c r="E198" s="11" t="s">
         <v>274</v>
@@ -3901,7 +3901,7 @@
       <c r="G198" s="6"/>
       <c r="H198" s="6"/>
     </row>
-    <row r="199" spans="4:8">
+    <row r="199" spans="4:8" x14ac:dyDescent="0.35">
       <c r="E199" s="17" t="s">
         <v>275</v>
       </c>
@@ -3933,36 +3933,53 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Government_x0020_Body xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">BEIS</Government_x0020_Body>
-    <Date_x0020_Opened xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">2023-10-25T11:25:00+00:00</Date_x0020_Opened>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6cb35823-445c-4345-bb19-437b7a53ef29">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <LegacyData xmlns="aaacb922-5235-4a66-b188-303b9b46fbd7" xsi:nil="true"/>
-    <Descriptor xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f" xsi:nil="true"/>
-    <Security_x0020_Classification xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f">OFFICIAL</Security_x0020_Classification>
-    <TaxCatchAll xmlns="6e2ffcde-8175-4cfa-8e98-1eddac4a692a">
-      <Value>1</Value>
-    </TaxCatchAll>
-    <m975189f4ba442ecbf67d4147307b177 xmlns="6e2ffcde-8175-4cfa-8e98-1eddac4a692a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">BEIS:Market Frameworks:Office for Product Safety and Standards</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">ce37d5da-e07d-451f-b694-ebae85a28213</TermId>
-        </TermInfo>
-      </Terms>
-    </m975189f4ba442ecbf67d4147307b177>
-    <Retention_x0020_Label xmlns="a8f60570-4bd3-4f2b-950b-a996de8ab151" xsi:nil="true"/>
-    <Date_x0020_Closed xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
-    <_dlc_DocId xmlns="6e2ffcde-8175-4cfa-8e98-1eddac4a692a">TK5FE52DNWW3-504769661-1124554</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="6e2ffcde-8175-4cfa-8e98-1eddac4a692a">
-      <Url>https://beisgov.sharepoint.com/sites/OPSSDT2/_layouts/15/DocIdRedir.aspx?ID=TK5FE52DNWW3-504769661-1124554</Url>
-      <Description>TK5FE52DNWW3-504769661-1124554</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4333,67 +4350,88 @@
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Government_x0020_Body xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">BEIS</Government_x0020_Body>
+    <Date_x0020_Opened xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">2023-10-25T11:25:00+00:00</Date_x0020_Opened>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6cb35823-445c-4345-bb19-437b7a53ef29">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <LegacyData xmlns="aaacb922-5235-4a66-b188-303b9b46fbd7" xsi:nil="true"/>
+    <Descriptor xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f" xsi:nil="true"/>
+    <Security_x0020_Classification xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f">OFFICIAL</Security_x0020_Classification>
+    <TaxCatchAll xmlns="6e2ffcde-8175-4cfa-8e98-1eddac4a692a">
+      <Value>1</Value>
+    </TaxCatchAll>
+    <m975189f4ba442ecbf67d4147307b177 xmlns="6e2ffcde-8175-4cfa-8e98-1eddac4a692a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">BEIS:Market Frameworks:Office for Product Safety and Standards</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">ce37d5da-e07d-451f-b694-ebae85a28213</TermId>
+        </TermInfo>
+      </Terms>
+    </m975189f4ba442ecbf67d4147307b177>
+    <Retention_x0020_Label xmlns="a8f60570-4bd3-4f2b-950b-a996de8ab151" xsi:nil="true"/>
+    <Date_x0020_Closed xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
+    <_dlc_DocId xmlns="6e2ffcde-8175-4cfa-8e98-1eddac4a692a">TK5FE52DNWW3-504769661-1124554</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="6e2ffcde-8175-4cfa-8e98-1eddac4a692a">
+      <Url>https://beisgov.sharepoint.com/sites/OPSSDT2/_layouts/15/DocIdRedir.aspx?ID=TK5FE52DNWW3-504769661-1124554</Url>
+      <Description>TK5FE52DNWW3-504769661-1124554</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{260BFBB0-A7F4-4BD3-928C-4C04CDD84D99}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{260BFBB0-A7F4-4BD3-928C-4C04CDD84D99}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6451A11E-A4A2-48F4-B504-5DFCC53D6385}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{680E353F-568D-4B5D-A032-06EAFF3D6C5F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3CD62E41-456A-454F-BD71-7411BF4002A3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3CD62E41-456A-454F-BD71-7411BF4002A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6e2ffcde-8175-4cfa-8e98-1eddac4a692a"/>
+    <ds:schemaRef ds:uri="0063f72e-ace3-48fb-9c1f-5b513408b31f"/>
+    <ds:schemaRef ds:uri="b413c3fd-5a3b-4239-b985-69032e371c04"/>
+    <ds:schemaRef ds:uri="a8f60570-4bd3-4f2b-950b-a996de8ab151"/>
+    <ds:schemaRef ds:uri="aaacb922-5235-4a66-b188-303b9b46fbd7"/>
+    <ds:schemaRef ds:uri="6cb35823-445c-4345-bb19-437b7a53ef29"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{680E353F-568D-4B5D-A032-06EAFF3D6C5F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6451A11E-A4A2-48F4-B504-5DFCC53D6385}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b413c3fd-5a3b-4239-b985-69032e371c04"/>
+    <ds:schemaRef ds:uri="6cb35823-445c-4345-bb19-437b7a53ef29"/>
+    <ds:schemaRef ds:uri="aaacb922-5235-4a66-b188-303b9b46fbd7"/>
+    <ds:schemaRef ds:uri="0063f72e-ace3-48fb-9c1f-5b513408b31f"/>
+    <ds:schemaRef ds:uri="6e2ffcde-8175-4cfa-8e98-1eddac4a692a"/>
+    <ds:schemaRef ds:uri="a8f60570-4bd3-4f2b-950b-a996de8ab151"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>